<commit_message>
Adicionar formato csv do arquivo "Nutrição" que contém medidas
</commit_message>
<xml_diff>
--- a/workout-nutrition/Nutrição.xlsx
+++ b/workout-nutrition/Nutrição.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteris1-my.sharepoint.com/personal/andressa_silva_iteris_com_br/Documents/GitHub/data-analysis/workout-nutrition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andressa.silva\Documents\GitHub\data-analysis\workout-nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B6F4BA-7332-4747-9E2C-97493CD00B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639F9BD7-68BC-4DD7-AF42-DC0274B4D52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9094E284-37DC-4DC0-8A01-64760B0F64C2}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Altura</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Bíceps esquerdo</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +213,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -223,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,6 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,7 +1337,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,6 +1396,9 @@
     </row>
     <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="B5" s="1">
         <v>44873</v>
       </c>

</xml_diff>

<commit_message>
Alteração dos arquivos para adição de fase 1 e 2 em formato CSV
</commit_message>
<xml_diff>
--- a/workout-nutrition/Nutrição.xlsx
+++ b/workout-nutrition/Nutrição.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andressa.silva\Documents\GitHub\data-analysis\workout-nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639F9BD7-68BC-4DD7-AF42-DC0274B4D52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9950FD6E-6CD1-472B-9535-CD1549331106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9094E284-37DC-4DC0-8A01-64760B0F64C2}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>tc={BC5AF60B-75EF-43C5-96D8-7352A360D633}</author>
   </authors>
   <commentList>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{BC5AF60B-75EF-43C5-96D8-7352A360D633}">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{BC5AF60B-75EF-43C5-96D8-7352A360D633}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Altura</t>
   </si>
@@ -66,51 +66,6 @@
     <t>Nascimento</t>
   </si>
   <si>
-    <t>ANDRESSA SOARES LIMA SILVA</t>
-  </si>
-  <si>
-    <t>Cintura</t>
-  </si>
-  <si>
-    <t>Abdômen</t>
-  </si>
-  <si>
-    <t>Quadril</t>
-  </si>
-  <si>
-    <t>Coxa esquerda</t>
-  </si>
-  <si>
-    <t>Coxa direita</t>
-  </si>
-  <si>
-    <t>Braço relaxado esquerdo</t>
-  </si>
-  <si>
-    <t>Braço relaxado direito</t>
-  </si>
-  <si>
-    <t>Tríceps</t>
-  </si>
-  <si>
-    <t>Abdominal</t>
-  </si>
-  <si>
-    <t>Axilar média</t>
-  </si>
-  <si>
-    <t>Suprailíaca</t>
-  </si>
-  <si>
-    <t>Subescapular</t>
-  </si>
-  <si>
-    <t>Torax</t>
-  </si>
-  <si>
-    <t>Coxa</t>
-  </si>
-  <si>
     <t>PESO</t>
   </si>
   <si>
@@ -132,34 +87,76 @@
     <t>Razão Cintura/Quadril</t>
   </si>
   <si>
-    <t>Dobras (mm)</t>
-  </si>
-  <si>
-    <t>Circunf. (mm)</t>
-  </si>
-  <si>
-    <t>Braço contraido esquerdo</t>
-  </si>
-  <si>
-    <t>Braço contraido direito</t>
-  </si>
-  <si>
-    <t>Tórax</t>
-  </si>
-  <si>
-    <t>Tríceps direito</t>
-  </si>
-  <si>
-    <t>Tríceps esquerdo</t>
-  </si>
-  <si>
-    <t>Bíceps direito</t>
-  </si>
-  <si>
-    <t>Bíceps esquerdo</t>
-  </si>
-  <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>(c) Cintura</t>
+  </si>
+  <si>
+    <t>(c) Abdômen</t>
+  </si>
+  <si>
+    <t>(c) Quadril</t>
+  </si>
+  <si>
+    <t>(c) Coxa esquerda</t>
+  </si>
+  <si>
+    <t>(c) Coxa direita</t>
+  </si>
+  <si>
+    <t>(c) Braço relaxado esquerdo</t>
+  </si>
+  <si>
+    <t>(c) Braço relaxado direito</t>
+  </si>
+  <si>
+    <t>(d) Tríceps</t>
+  </si>
+  <si>
+    <t>(d) Abdominal</t>
+  </si>
+  <si>
+    <t>(d) Axilar média</t>
+  </si>
+  <si>
+    <t>(d) Suprailíaca</t>
+  </si>
+  <si>
+    <t>(d) Subescapular</t>
+  </si>
+  <si>
+    <t>(d) Torax</t>
+  </si>
+  <si>
+    <t>(d) Coxa</t>
+  </si>
+  <si>
+    <t>(c) Braço contraido esquerdo</t>
+  </si>
+  <si>
+    <t>(c) Braço contraido direito</t>
+  </si>
+  <si>
+    <t>(c) Tórax</t>
+  </si>
+  <si>
+    <t>(d) Tríceps direito</t>
+  </si>
+  <si>
+    <t>(d) Tríceps esquerdo</t>
+  </si>
+  <si>
+    <t>(d) Bíceps direito</t>
+  </si>
+  <si>
+    <t>(d) Bíceps esquerdo</t>
+  </si>
+  <si>
+    <t>(d) Coxa direita</t>
+  </si>
+  <si>
+    <t>(d) Coxa esquerda</t>
   </si>
 </sst>
 </file>
@@ -232,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -242,9 +239,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +560,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I13" dT="2022-10-18T23:29:35.72" personId="{4DA6E33C-6015-45B4-9494-A0B70B4E1606}" id="{BC5AF60B-75EF-43C5-96D8-7352A360D633}">
+  <threadedComment ref="I12" dT="2022-10-18T23:29:35.72" personId="{4DA6E33C-6015-45B4-9494-A0B70B4E1606}" id="{BC5AF60B-75EF-43C5-96D8-7352A360D633}">
     <text>Não houve dado no dietbox</text>
   </threadedComment>
 </ThreadedComments>
@@ -574,13 +568,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A02D1E7-67C6-4A43-AF89-AFD62FAB2002}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,360 +587,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>25</v>
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>35468</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>35468</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>163</v>
+      </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>163</v>
-      </c>
-      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
-        <f ca="1" xml:space="preserve"> YEAR(TODAY())-YEAR(B2)</f>
+      <c r="E2" s="3">
+        <f ca="1" xml:space="preserve"> YEAR(TODAY())-YEAR(B1)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+    <row r="3" spans="1:15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
         <v>44617</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C4" s="1">
         <v>44636</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D4" s="1">
         <v>44671</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E4" s="1">
         <v>44705</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F4" s="1">
         <v>44732</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G4" s="1">
         <v>44793</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H4" s="1">
         <v>44824</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I4" s="1">
         <v>44849</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J4" s="1">
         <v>44869</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>88.1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>85.8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>85.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>82.7</v>
+      </c>
+      <c r="F5" s="2">
+        <v>84.6</v>
+      </c>
+      <c r="G5" s="2">
+        <v>84.5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>84.5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>84.4</v>
+      </c>
+      <c r="J5" s="2">
+        <v>85.4</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>88.1</v>
+        <f>B5*10000/POWER($B$2,2)</f>
+        <v>33.158944634724676</v>
       </c>
       <c r="C6" s="2">
-        <v>85.8</v>
+        <f>C5*10000/POWER($B$2,2)</f>
+        <v>32.293274116451506</v>
       </c>
       <c r="D6" s="2">
-        <v>85.5</v>
+        <f t="shared" ref="D6:J6" si="0">D5*10000/POWER($B$2,2)</f>
+        <v>32.180360570589784</v>
       </c>
       <c r="E6" s="2">
-        <v>82.7</v>
+        <f t="shared" si="0"/>
+        <v>31.126500809213745</v>
       </c>
       <c r="F6" s="2">
-        <v>84.6</v>
+        <f t="shared" si="0"/>
+        <v>31.84161993300463</v>
       </c>
       <c r="G6" s="2">
-        <v>84.5</v>
+        <f t="shared" si="0"/>
+        <v>31.803982084384057</v>
       </c>
       <c r="H6" s="2">
-        <v>84.5</v>
+        <f t="shared" si="0"/>
+        <v>31.803982084384057</v>
       </c>
       <c r="I6" s="2">
-        <v>84.4</v>
+        <f t="shared" si="0"/>
+        <v>31.766344235763484</v>
       </c>
       <c r="J6" s="2">
-        <v>85.4</v>
+        <f t="shared" si="0"/>
+        <v>32.142722721969214</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <f>B6*10000/POWER($B$3,2)</f>
-        <v>33.158944634724676</v>
+        <f ca="1">1.112-0.00043499*(B23)+ 0.00000055*(B23)*2-0.00028826*($E$2)</f>
+        <v>1.0076021400000001</v>
       </c>
       <c r="C7" s="2">
-        <f>C6*10000/POWER($B$3,2)</f>
-        <v>32.293274116451506</v>
+        <f t="shared" ref="C7:J7" ca="1" si="1">1.112-0.00043499*(C23)+ 0.00000055*(C23)*2-0.00028826*($E$2)</f>
+        <v>1.0184493900000002</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:J7" si="0">D6*10000/POWER($B$3,2)</f>
-        <v>32.180360570589784</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0249577400000003</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>31.126500809213745</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0245238500000002</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>31.84161993300463</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0214866200000003</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>31.803982084384057</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0318999800000002</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>31.803982084384057</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0318999800000002</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>31.766344235763484</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0336355400000004</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="0"/>
-        <v>32.142722721969214</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0345033200000002</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <f ca="1">1.112-0.00043499*(B24)+ 0.00000055*(B24)*2-0.00028826*($E$3)</f>
-        <v>1.0076021400000001</v>
+        <f t="shared" ref="B8:F8" si="2">B9/B11</f>
+        <v>0.83898305084745761</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:J8" ca="1" si="1">1.112-0.00043499*(C24)+ 0.00000055*(C24)*2-0.00028826*($E$3)</f>
-        <v>1.0184493900000002</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0249577400000003</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0245238500000002</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0214866200000003</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0318999800000002</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0318999800000002</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0336355400000004</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0345033200000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <f t="shared" ref="B9:F9" si="2">B10/B12</f>
-        <v>0.83898305084745761</v>
-      </c>
-      <c r="C9" s="2">
         <f t="shared" si="2"/>
         <v>0.86842105263157898</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D8" s="2">
         <f t="shared" si="2"/>
         <v>0.76991150442477874</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
         <v>0.75221238938053092</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F8" s="2">
         <f t="shared" si="2"/>
         <v>0.81578947368421051</v>
       </c>
-      <c r="G9" s="2">
-        <f>G10/G12</f>
+      <c r="G8" s="2">
+        <f>G9/G11</f>
         <v>0.83620689655172409</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" ref="H9:J9" si="3">H10/H12</f>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:J8" si="3">H9/H11</f>
         <v>0.82758620689655171</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I8" s="2">
         <f t="shared" si="3"/>
         <v>0.81196581196581197</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J8" s="2">
         <f t="shared" si="3"/>
         <v>0.83620689655172409</v>
       </c>
     </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>99</v>
+      </c>
+      <c r="C9" s="2">
+        <v>99</v>
+      </c>
+      <c r="D9" s="2">
+        <v>87</v>
+      </c>
+      <c r="E9" s="2">
+        <v>85</v>
+      </c>
+      <c r="F9" s="2">
+        <v>93</v>
+      </c>
+      <c r="G9" s="2">
+        <v>97</v>
+      </c>
+      <c r="H9" s="2">
+        <v>96</v>
+      </c>
+      <c r="I9" s="2">
+        <v>95</v>
+      </c>
+      <c r="J9" s="2">
+        <v>97</v>
+      </c>
+    </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C10" s="2">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D10" s="2">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="G10" s="2">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="H10" s="2">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="I10" s="2">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="J10" s="2">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D11" s="2">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E11" s="2">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F11" s="2">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="G11" s="2">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="H11" s="2">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I11" s="2">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="J11" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="H12" s="2">
-        <v>116</v>
-      </c>
-      <c r="I12" s="2">
-        <v>117</v>
+        <v>57</v>
+      </c>
+      <c r="I12" s="7">
+        <v>56</v>
       </c>
       <c r="J12" s="2">
-        <v>116</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2">
+        <v>55.5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2">
         <v>56</v>
       </c>
-      <c r="C13" s="2">
-        <v>58</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="H13" s="2">
         <v>55</v>
-      </c>
-      <c r="E13" s="2">
-        <v>55</v>
-      </c>
-      <c r="F13" s="2">
-        <v>56</v>
-      </c>
-      <c r="G13" s="2">
-        <v>57</v>
-      </c>
-      <c r="H13" s="2">
-        <v>57</v>
       </c>
       <c r="I13" s="7">
         <v>56</v>
@@ -957,39 +971,39 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2">
-        <v>55.5</v>
+        <v>31</v>
       </c>
       <c r="F14" s="2">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="G14" s="2">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2">
-        <v>55</v>
-      </c>
-      <c r="I14" s="7">
-        <v>56</v>
+        <v>32</v>
+      </c>
+      <c r="I14" s="2">
+        <v>31</v>
       </c>
       <c r="J14" s="2">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <v>34</v>
@@ -1001,16 +1015,16 @@
         <v>32</v>
       </c>
       <c r="E15" s="2">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2">
         <v>31</v>
       </c>
-      <c r="F15" s="2">
-        <v>32</v>
-      </c>
       <c r="G15" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H15" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="2">
         <v>31</v>
@@ -1020,310 +1034,275 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>10</v>
+      <c r="A16" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F16" s="2">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H16" s="2">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="I16" s="2">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J16" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E17" s="2">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F17" s="2">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H17" s="2">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="I17" s="2">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="J17" s="2">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>35</v>
       </c>
       <c r="D18" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2">
         <v>33</v>
       </c>
       <c r="F18" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I18" s="2">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J18" s="2">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E19" s="2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F19" s="2">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G19" s="2">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2">
         <v>30</v>
       </c>
-      <c r="H19" s="2">
-        <v>27</v>
-      </c>
       <c r="I19" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J19" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D20" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E20" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F20" s="2">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G20" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I20" s="2">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J20" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E21" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F21" s="2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G21" s="2">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H21" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I21" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J21" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>35</v>
+      </c>
+      <c r="C22" s="2">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2">
+        <v>26</v>
+      </c>
+      <c r="E22" s="2">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2">
+        <v>25</v>
+      </c>
+      <c r="G22" s="2">
+        <v>25</v>
+      </c>
+      <c r="H22" s="2">
+        <v>20</v>
+      </c>
+      <c r="I22" s="2">
         <v>16</v>
       </c>
-      <c r="B22" s="2">
-        <v>30</v>
-      </c>
-      <c r="C22" s="2">
-        <v>24</v>
-      </c>
-      <c r="D22" s="2">
-        <v>17</v>
-      </c>
-      <c r="E22" s="2">
-        <v>23</v>
-      </c>
-      <c r="F22" s="2">
-        <v>23</v>
-      </c>
-      <c r="G22" s="2">
-        <v>16</v>
-      </c>
-      <c r="H22" s="2">
-        <v>17</v>
-      </c>
-      <c r="I22" s="2">
-        <v>17</v>
-      </c>
       <c r="J22" s="2">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>17</v>
+      <c r="A23" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B23" s="2">
-        <v>35</v>
+        <f>SUM(B16:B22)</f>
+        <v>224</v>
       </c>
       <c r="C23" s="2">
-        <v>30</v>
+        <f t="shared" ref="C23:J23" si="4">SUM(C16:C22)</f>
+        <v>199</v>
       </c>
       <c r="D23" s="2">
-        <v>26</v>
-      </c>
-      <c r="E23" s="2">
-        <v>25</v>
-      </c>
-      <c r="F23" s="2">
-        <v>25</v>
-      </c>
-      <c r="G23" s="2">
-        <v>25</v>
-      </c>
-      <c r="H23" s="2">
-        <v>20</v>
-      </c>
-      <c r="I23" s="2">
-        <v>16</v>
-      </c>
-      <c r="J23" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2">
-        <f>SUM(B17:B23)</f>
-        <v>224</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" ref="C24:J24" si="4">SUM(C17:C23)</f>
-        <v>199</v>
-      </c>
-      <c r="D24" s="2">
         <f t="shared" si="4"/>
         <v>184</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E23" s="2">
         <f t="shared" si="4"/>
         <v>185</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F23" s="2">
         <f t="shared" si="4"/>
         <v>192</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G23" s="2">
         <f t="shared" si="4"/>
         <v>168</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H23" s="2">
         <f t="shared" si="4"/>
         <v>168</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I23" s="2">
         <f t="shared" si="4"/>
         <v>164</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J23" s="2">
         <f t="shared" si="4"/>
         <v>162</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B24 C24:I24" formulaRange="1"/>
+    <ignoredError sqref="B23 C23:I23" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -1331,13 +1310,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3331AF-6F1D-4ECB-BDE5-81D2DB25009F}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,240 +1329,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>25</v>
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>35468</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>35468</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>163</v>
+      </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>163</v>
-      </c>
-      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
-        <f ca="1" xml:space="preserve"> YEAR(TODAY())-YEAR(B2)</f>
+      <c r="E2" s="3">
+        <f ca="1" xml:space="preserve"> YEAR(TODAY())-YEAR(B1)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="3" spans="1:15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
         <v>44873</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>85.5</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>85.5</v>
+        <f>B5*10000/POWER($B$2,2)</f>
+        <v>32.180360570589784</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <f>B6*10000/POWER($B$3,2)</f>
-        <v>32.180360570589784</v>
+        <f ca="1">1.112-0.00043499*(B30)+ 0.00000055*(B30)*2-0.00028826*($E$2)</f>
+        <v>0.99545322000000003</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <f ca="1">1.112-0.00043499*(B31)+ 0.00000055*(B31)*2-0.00028826*($E$3)</f>
-        <v>0.99545322000000003</v>
+        <f>B9/B11</f>
+        <v>0.84782608695652173</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
+      <c r="A9" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="2">
-        <f>B10/B12</f>
-        <v>0.84782608695652173</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>97.5</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>115</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>60</v>
+        <v>60.5</v>
       </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>60.5</v>
-      </c>
-      <c r="I14" s="7"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>37</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2">
-        <v>37.5</v>
+        <v>35.799999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
-        <v>35.799999999999997</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="2">
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="B19" s="2">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2">
         <v>35</v>
@@ -1591,49 +1563,38 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="2">
-        <f>SUM(AVERAGE(B20:B21),AVERAGE(B22:B23),AVERAGE(B29:B30),B24:B28)</f>
+        <f>SUM(AVERAGE(B19:B20),AVERAGE(B21:B22),AVERAGE(B28:B29),B23:B27)</f>
         <v>252</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>